<commit_message>
Cambio de horario del Lunes 13/02
</commit_message>
<xml_diff>
--- a/Me programo.xlsx
+++ b/Me programo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E80C7BA-40F6-4427-82FA-A351D9E3C2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98B89EE-73E2-44C9-B5C0-260A65B28983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="51">
   <si>
     <t>Lunes 13</t>
   </si>
@@ -189,6 +189,13 @@
   <si>
     <t>Almorzar
 Ir a la Universidad</t>
+  </si>
+  <si>
+    <t>Arreglarse
+Desayunar</t>
+  </si>
+  <si>
+    <t>GYM</t>
   </si>
 </sst>
 </file>
@@ -293,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -303,8 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -602,9 +608,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AC22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F5" sqref="F5"/>
+      <selection pane="topRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,70 +639,70 @@
       <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="R2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="T2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Y2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="Z2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="14" t="s">
+      <c r="AA2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AB2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="AC2" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -704,88 +710,88 @@
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="X3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC3" s="9" t="s">
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -793,88 +799,88 @@
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="X4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC4" s="9" t="s">
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -882,88 +888,88 @@
       <c r="A5" s="4">
         <v>0.27777777777777779</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="10" t="s">
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="10" t="s">
+      <c r="K5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="10" t="s">
+      <c r="M5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S5" s="10" t="s">
+      <c r="R5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="T5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W5" s="10" t="s">
+      <c r="T5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="X5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Y5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z5" s="10" t="s">
+      <c r="Y5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AA5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AA5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -971,88 +977,88 @@
       <c r="A6" s="4">
         <v>0.29166666666666702</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="11" t="s">
+      <c r="M6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="11" t="s">
+      <c r="Q6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="R6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="R6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S6" s="11" t="s">
+      <c r="T6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="T6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="U6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W6" s="11" t="s">
+      <c r="X6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="Y6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Y6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z6" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC6" s="9" t="s">
+      <c r="AA6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1060,25 +1066,25 @@
       <c r="A7" s="4">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>32</v>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1087,19 +1093,19 @@
       <c r="J7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O7" s="9" t="s">
+      <c r="M7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P7" s="2" t="s">
@@ -1108,19 +1114,19 @@
       <c r="Q7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="R7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="S7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="T7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="U7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V7" s="9" t="s">
+      <c r="T7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="W7" s="2" t="s">
@@ -1129,19 +1135,19 @@
       <c r="X7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="Y7" s="9" t="s">
+      <c r="Y7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="Z7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AA7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC7" s="9" t="s">
+      <c r="AA7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1149,25 +1155,25 @@
       <c r="A8" s="4">
         <v>0.375</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>32</v>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1176,19 +1182,19 @@
       <c r="J8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="N8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="P8" s="2" t="s">
@@ -1197,19 +1203,19 @@
       <c r="Q8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="R8" s="11" t="s">
+      <c r="R8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="S8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="T8" s="11" t="s">
+      <c r="T8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="U8" s="11" t="s">
+      <c r="U8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V8" s="11" t="s">
+      <c r="V8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="W8" s="2" t="s">
@@ -1218,19 +1224,19 @@
       <c r="X8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="Y8" s="11" t="s">
+      <c r="Y8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="Z8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AA8" s="11" t="s">
+      <c r="AA8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AB8" s="11" t="s">
+      <c r="AB8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AC8" s="11" t="s">
+      <c r="AC8" s="10" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1327,8 +1333,8 @@
       <c r="A10" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>41</v>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>35</v>
@@ -1416,8 +1422,8 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>41</v>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
@@ -1505,88 +1511,88 @@
       <c r="A12" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="P12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="R12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="S12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="T12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="U12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="V12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="W12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="X12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC12" s="11" t="s">
+      <c r="B12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="V12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="W12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="X12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC12" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1951,7 +1957,7 @@
         <v>0.75</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>35</v>
@@ -2039,88 +2045,88 @@
       <c r="A18" s="4">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="R18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="S18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="T18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="U18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="V18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="W18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="X18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC18" s="12" t="s">
+      <c r="B18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="T18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="U18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="V18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="W18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="X18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC18" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2128,8 +2134,8 @@
       <c r="A19" s="4">
         <v>0.83333333333333304</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>35</v>
+      <c r="B19" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>35</v>
@@ -2217,8 +2223,8 @@
       <c r="A20" s="4">
         <v>0.875</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>35</v>
+      <c r="B20" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>40</v>
@@ -2306,13 +2312,13 @@
       <c r="A21" s="4">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -2324,16 +2330,16 @@
       <c r="G21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="9" t="s">
+      <c r="H21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L21" s="5" t="s">
@@ -2345,16 +2351,16 @@
       <c r="N21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O21" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P21" s="9" t="s">
+      <c r="O21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R21" s="9" t="s">
+      <c r="R21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="S21" s="5" t="s">
@@ -2366,16 +2372,16 @@
       <c r="U21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="V21" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W21" s="9" t="s">
+      <c r="V21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="X21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Y21" s="9" t="s">
+      <c r="Y21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="Z21" s="5" t="s">
@@ -2387,7 +2393,7 @@
       <c r="AB21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AC21" s="9" t="s">
+      <c r="AC21" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2395,88 +2401,88 @@
       <c r="A22" s="4">
         <v>0.95833333333333304</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="T22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="U22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="X22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC22" s="9" t="s">
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC22" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizacion de la semana 1
</commit_message>
<xml_diff>
--- a/Me programo.xlsx
+++ b/Me programo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98B89EE-73E2-44C9-B5C0-260A65B28983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8996C977-CAC4-48E4-8BC5-E6A5F01AB9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="53">
   <si>
     <t>Lunes 13</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>GYM</t>
+  </si>
+  <si>
+    <t>Ir a hacer mercado</t>
+  </si>
+  <si>
+    <t>Cocinar</t>
   </si>
 </sst>
 </file>
@@ -608,9 +614,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AC22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B9" sqref="B9"/>
+      <selection pane="topRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1254,7 +1260,7 @@
         <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>43</v>
@@ -1432,7 +1438,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>35</v>
@@ -1615,8 +1621,8 @@
       <c r="F13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>47</v>
+      <c r="G13" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>35</v>
@@ -1704,8 +1710,8 @@
       <c r="F14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>47</v>
+      <c r="G14" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>46</v>
@@ -1781,20 +1787,20 @@
       <c r="B15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>35</v>
+      <c r="G15" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>46</v>
@@ -1870,14 +1876,14 @@
       <c r="B16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>36</v>
+      <c r="C16" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>36</v>
+      <c r="E16" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>45</v>
@@ -1959,8 +1965,8 @@
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
+      <c r="C17" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>35</v>
@@ -2048,8 +2054,8 @@
       <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>34</v>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>34</v>
@@ -2138,10 +2144,10 @@
         <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>35</v>
@@ -2149,8 +2155,8 @@
       <c r="F19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>41</v>
+      <c r="G19" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>35</v>
@@ -2226,11 +2232,11 @@
       <c r="B20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>41</v>
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>40</v>
@@ -2238,8 +2244,8 @@
       <c r="F20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>41</v>
+      <c r="G20" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>35</v>
@@ -2315,11 +2321,11 @@
       <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>40</v>
+      <c r="C21" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>40</v>
@@ -2404,8 +2410,8 @@
       <c r="B22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
+      <c r="C22" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Actualizacion de Lunes 20 y martes 21
</commit_message>
<xml_diff>
--- a/Me programo.xlsx
+++ b/Me programo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8996C977-CAC4-48E4-8BC5-E6A5F01AB9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE47D711-05A0-4D39-BFCD-019E9CEEB920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="55">
   <si>
     <t>Lunes 13</t>
   </si>
@@ -202,6 +202,13 @@
   </si>
   <si>
     <t>Cocinar</t>
+  </si>
+  <si>
+    <t>Lavar ropa</t>
+  </si>
+  <si>
+    <t>Informatica II: 
+Practica 1</t>
   </si>
 </sst>
 </file>
@@ -223,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +285,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -306,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -325,6 +338,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -333,9 +350,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFB07BD7"/>
       <color rgb="FFFF8585"/>
       <color rgb="FFD6D6FE"/>
-      <color rgb="FFB07BD7"/>
     </mruColors>
   </colors>
   <extLst>
@@ -614,9 +631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AC22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1335,7 +1352,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>0.45833333333333298</v>
       </c>
@@ -1360,11 +1377,11 @@
       <c r="H10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>41</v>
+      <c r="I10" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>43</v>
@@ -1449,11 +1466,11 @@
       <c r="H11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>41</v>
+      <c r="I11" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>35</v>
@@ -1897,8 +1914,8 @@
       <c r="I16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>36</v>
+      <c r="J16" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>45</v>
@@ -1986,8 +2003,8 @@
       <c r="I17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>35</v>
+      <c r="J17" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>35</v>
@@ -2075,8 +2092,8 @@
       <c r="I18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="11" t="s">
-        <v>34</v>
+      <c r="J18" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="K18" s="11" t="s">
         <v>34</v>
@@ -2161,11 +2178,11 @@
       <c r="H19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>35</v>
+      <c r="I19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>46</v>

</xml_diff>